<commit_message>
update institutions - add CESNET
</commit_message>
<xml_diff>
--- a/data/excel/institutions.xlsx
+++ b/data/excel/institutions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14880" windowHeight="7464" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="slovník" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10293" uniqueCount="4223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10301" uniqueCount="4228">
   <si>
     <t>code</t>
   </si>
@@ -12699,6 +12699,21 @@
   </si>
   <si>
     <t>polytechnique-montreal</t>
+  </si>
+  <si>
+    <t>cesnet</t>
+  </si>
+  <si>
+    <t>CESNET</t>
+  </si>
+  <si>
+    <t>https://ror.org/050dkka69</t>
+  </si>
+  <si>
+    <t>Czech Education and Scientific Network</t>
+  </si>
+  <si>
+    <t>https://www.cesnet.cz</t>
   </si>
 </sst>
 </file>
@@ -13207,9 +13222,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK1802"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A1782" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1788" sqref="A1788:XFD1788"/>
+      <selection pane="bottomLeft" activeCell="A1792" sqref="A1792"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -73358,22 +73373,43 @@
       <c r="AE1791" s="19"/>
     </row>
     <row r="1792" spans="1:31" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1792" s="19"/>
-      <c r="B1792" s="19"/>
-      <c r="C1792"/>
+      <c r="A1792" s="19">
+        <v>1</v>
+      </c>
+      <c r="B1792" s="19" t="s">
+        <v>4223</v>
+      </c>
+      <c r="C1792" t="s">
+        <v>4224</v>
+      </c>
       <c r="D1792" s="19"/>
-      <c r="E1792" s="19"/>
-      <c r="G1792" s="19"/>
+      <c r="E1792" s="19" t="s">
+        <v>4224</v>
+      </c>
+      <c r="G1792" s="19" t="s">
+        <v>3619</v>
+      </c>
       <c r="H1792" s="19"/>
+      <c r="I1792" s="8" t="s">
+        <v>4226</v>
+      </c>
       <c r="J1792" s="19"/>
       <c r="K1792" s="19"/>
       <c r="M1792" s="19"/>
       <c r="N1792" s="19"/>
-      <c r="O1792" s="3"/>
-      <c r="P1792" s="19"/>
-      <c r="Q1792" s="19"/>
+      <c r="O1792" s="17">
+        <v>63839172</v>
+      </c>
+      <c r="P1792" s="22" t="s">
+        <v>4225</v>
+      </c>
+      <c r="Q1792" s="19" t="s">
+        <v>4227</v>
+      </c>
       <c r="S1792" s="19"/>
-      <c r="T1792" s="19"/>
+      <c r="T1792" s="19" t="s">
+        <v>3658</v>
+      </c>
       <c r="V1792" s="19"/>
       <c r="W1792" s="19"/>
       <c r="Y1792" s="19"/>
@@ -73666,9 +73702,10 @@
     <hyperlink ref="P1789" r:id="rId16"/>
     <hyperlink ref="P1790" r:id="rId17"/>
     <hyperlink ref="P1791" r:id="rId18"/>
+    <hyperlink ref="P1792" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -73676,7 +73713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>